<commit_message>
took out bad vibes form chart
</commit_message>
<xml_diff>
--- a/speed.xlsx
+++ b/speed.xlsx
@@ -195,7 +195,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.0676171333826439"/>
-          <c:y val="0.13518191430448"/>
+          <c:y val="0.127107148329636"/>
           <c:w val="0.898958475089628"/>
           <c:h val="0.782246927615127"/>
         </c:manualLayout>
@@ -204,378 +204,8 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet2!$A$5:$A$56</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="52"/>
-                <c:pt idx="0">
-                  <c:v>-255.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-245.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-235.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-225.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-215.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-205.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-195.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-185.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-175.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-165.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-155.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-145.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-135.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-125.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-115.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-105.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-95.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-85.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-75.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-65.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-55.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-45.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-35.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-25.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-15.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-5.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>35.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>45.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>65.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>95.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>105.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>115.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>125.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>135.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>145.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>155.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>165.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>175.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>185.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>195.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>205.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>215.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>225.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>235.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>245.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>255.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet2!$B$5:$B$56</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="52"/>
-                <c:pt idx="0">
-                  <c:v>4.936363636363636</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.875</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.864285714285714</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.03921568627451</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.893048128342246</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.37984496124031</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.865853658536585</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.532994923857868</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.126865671641791</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.579457364341085</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.0835</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.0335</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.0295</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.0255</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.023</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.016</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.013</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.0075</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.0065</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.0045</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.003</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.0015</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.001</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.003</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.0085</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.013</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.0144927536231884</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.0165</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.0175</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.019</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.0215</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.0335</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.205</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.21</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet2!$C$4</c:f>
@@ -945,7 +575,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet2!$D$4</c:f>
@@ -1307,376 +937,6 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>3.901960784313725</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet2!$A$5:$A$56</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="52"/>
-                <c:pt idx="0">
-                  <c:v>-255.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-245.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-235.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-225.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-215.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-205.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-195.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-185.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-175.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-165.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-155.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-145.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-135.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-125.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-115.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-105.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-95.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-85.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-75.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-65.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-55.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-45.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-35.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-25.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-15.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-5.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>35.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>45.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>65.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>95.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>105.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>115.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>125.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>135.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>145.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>155.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>165.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>175.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>185.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>195.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>205.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>215.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>225.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>235.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>245.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>255.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet2!$E$5:$E$56</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="52"/>
-                <c:pt idx="0">
-                  <c:v>6.934782608695652</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.5390625</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.700636942675159</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.371549893842887</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.636986301369863</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0265</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.141</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.063</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.049</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.0425</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.0115</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.0065</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.0055</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.0035</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.003</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.002</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.0025</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.001</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.0015</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.0005</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.001</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.001</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.001</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.001</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.001</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.001</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.0015</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.0015</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.002</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.0025</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.004</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.014</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.0345</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.0995</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.1175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5142,7 +4402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F57"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -6305,7 +5565,7 @@
   <dimension ref="A1:G209"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScaleNormal="39" zoomScalePageLayoutView="39" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>